<commit_message>
Besprechung in Stunden doku eingetragen
</commit_message>
<xml_diff>
--- a/ITP_Dokumente/STUNDEN DOKUMENTATION.xlsx
+++ b/ITP_Dokumente/STUNDEN DOKUMENTATION.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bjorn\Documents\fh 16-17\itp\TimeAid\ITP_Dokumente\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miel\Documents\FH\SS17\ITP\TimeAid\ITP_Dokumente\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>DATUM</t>
   </si>
@@ -82,6 +82,12 @@
   </si>
   <si>
     <t>Bjorna</t>
+  </si>
+  <si>
+    <t>16:00-17:00</t>
+  </si>
+  <si>
+    <t>4. Teambesprechung (Spezifikation)</t>
   </si>
 </sst>
 </file>
@@ -466,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F64"/>
+  <dimension ref="A1:F65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1"/>
@@ -599,36 +605,48 @@
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1">
       <c r="A7" s="3">
+        <v>42821</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="10">
+        <v>4</v>
+      </c>
+      <c r="E7" s="2">
+        <v>2</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A8" s="3">
         <v>42828</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D8" s="10">
         <v>1</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E8" s="9">
         <v>0.10416666666666667</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A8" s="3"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:6" ht="15.75" customHeight="1">
       <c r="A9" s="3"/>
       <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
+      <c r="C9" s="4"/>
       <c r="D9" s="10"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -701,7 +719,7 @@
       <c r="A18" s="3"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
-      <c r="D18" s="5"/>
+      <c r="D18" s="10"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
@@ -729,7 +747,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="1:6" ht="12.5">
+    <row r="22" spans="1:6" ht="15.75" customHeight="1">
       <c r="A22" s="3"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -786,7 +804,7 @@
       <c r="F28" s="2"/>
     </row>
     <row r="29" spans="1:6" ht="12.5">
-      <c r="A29" s="6"/>
+      <c r="A29" s="3"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="5"/>
@@ -810,7 +828,7 @@
       <c r="F31" s="2"/>
     </row>
     <row r="32" spans="1:6" ht="12.5">
-      <c r="A32" s="3"/>
+      <c r="A32" s="6"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="5"/>
@@ -986,7 +1004,7 @@
       <c r="F53" s="2"/>
     </row>
     <row r="54" spans="1:6" ht="12.5">
-      <c r="A54" s="2"/>
+      <c r="A54" s="3"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="5"/>
@@ -994,7 +1012,7 @@
       <c r="F54" s="2"/>
     </row>
     <row r="55" spans="1:6" ht="12.5">
-      <c r="A55" s="7"/>
+      <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="5"/>
@@ -1050,7 +1068,7 @@
       <c r="F61" s="2"/>
     </row>
     <row r="62" spans="1:6" ht="12.5">
-      <c r="A62" s="3"/>
+      <c r="A62" s="7"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="5"/>
@@ -1058,7 +1076,7 @@
       <c r="F62" s="2"/>
     </row>
     <row r="63" spans="1:6" ht="12.5">
-      <c r="A63" s="7"/>
+      <c r="A63" s="3"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
       <c r="D63" s="5"/>
@@ -1073,6 +1091,14 @@
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
     </row>
+    <row r="65" spans="1:6" ht="12.5">
+      <c r="A65" s="7"/>
+      <c r="B65" s="2"/>
+      <c r="C65" s="2"/>
+      <c r="D65" s="5"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>